<commit_message>
updated visualization descriptions, added legacy models, added results section
</commit_message>
<xml_diff>
--- a/ML Gantt Chart.xlsx
+++ b/ML Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushaldudipala/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushaldudipala/codebase/end me/CS4641-final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74C745A-A320-024A-9339-E14679ABA464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411EF3EB-DC32-A244-8A60-F790FC3DAE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
     <numFmt numFmtId="164" formatCode="mmm\ d"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -289,8 +289,14 @@
       <color rgb="FFBFBFBF"/>
       <name val="Corbel"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Corbel"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +427,24 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FFFCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor rgb="FFEDEDED"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -688,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -790,19 +814,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -824,24 +857,27 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,7 +1100,7 @@
   <dimension ref="A1:CF1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BA21" sqref="BA21"/>
+      <selection activeCell="BU31" sqref="BU31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1084,13 +1120,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="77"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1107,16 +1143,16 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="67" t="s">
+      <c r="AA1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
+      <c r="AB1" s="79"/>
+      <c r="AC1" s="79"/>
+      <c r="AD1" s="79"/>
+      <c r="AE1" s="79"/>
+      <c r="AF1" s="79"/>
+      <c r="AG1" s="79"/>
+      <c r="AH1" s="79"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
@@ -1259,12 +1295,12 @@
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="82"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1409,226 +1445,226 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="61"/>
-      <c r="U5" s="73" t="s">
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="60"/>
-      <c r="W5" s="60"/>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="60"/>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60"/>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="60"/>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="60"/>
-      <c r="AI5" s="60"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60"/>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60"/>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="60"/>
-      <c r="AR5" s="60"/>
-      <c r="AS5" s="60"/>
-      <c r="AT5" s="60"/>
-      <c r="AU5" s="60"/>
-      <c r="AV5" s="60"/>
-      <c r="AW5" s="60"/>
-      <c r="AX5" s="60"/>
-      <c r="AY5" s="60"/>
-      <c r="AZ5" s="60"/>
-      <c r="BA5" s="60"/>
-      <c r="BB5" s="60"/>
-      <c r="BC5" s="61"/>
-      <c r="BD5" s="74" t="s">
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="72"/>
+      <c r="Y5" s="72"/>
+      <c r="Z5" s="72"/>
+      <c r="AA5" s="72"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="72"/>
+      <c r="AE5" s="72"/>
+      <c r="AF5" s="72"/>
+      <c r="AG5" s="72"/>
+      <c r="AH5" s="72"/>
+      <c r="AI5" s="72"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="72"/>
+      <c r="AL5" s="72"/>
+      <c r="AM5" s="72"/>
+      <c r="AN5" s="72"/>
+      <c r="AO5" s="72"/>
+      <c r="AP5" s="72"/>
+      <c r="AQ5" s="72"/>
+      <c r="AR5" s="72"/>
+      <c r="AS5" s="72"/>
+      <c r="AT5" s="72"/>
+      <c r="AU5" s="72"/>
+      <c r="AV5" s="72"/>
+      <c r="AW5" s="72"/>
+      <c r="AX5" s="72"/>
+      <c r="AY5" s="72"/>
+      <c r="AZ5" s="72"/>
+      <c r="BA5" s="72"/>
+      <c r="BB5" s="72"/>
+      <c r="BC5" s="73"/>
+      <c r="BD5" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="BE5" s="60"/>
-      <c r="BF5" s="60"/>
-      <c r="BG5" s="60"/>
-      <c r="BH5" s="60"/>
-      <c r="BI5" s="60"/>
-      <c r="BJ5" s="60"/>
-      <c r="BK5" s="60"/>
-      <c r="BL5" s="60"/>
-      <c r="BM5" s="60"/>
-      <c r="BN5" s="60"/>
-      <c r="BO5" s="60"/>
-      <c r="BP5" s="60"/>
-      <c r="BQ5" s="60"/>
-      <c r="BR5" s="60"/>
-      <c r="BS5" s="60"/>
-      <c r="BT5" s="60"/>
-      <c r="BU5" s="60"/>
-      <c r="BV5" s="60"/>
-      <c r="BW5" s="60"/>
-      <c r="BX5" s="60"/>
-      <c r="BY5" s="60"/>
-      <c r="BZ5" s="60"/>
-      <c r="CA5" s="60"/>
-      <c r="CB5" s="60"/>
-      <c r="CC5" s="60"/>
-      <c r="CD5" s="60"/>
-      <c r="CE5" s="61"/>
+      <c r="BE5" s="72"/>
+      <c r="BF5" s="72"/>
+      <c r="BG5" s="72"/>
+      <c r="BH5" s="72"/>
+      <c r="BI5" s="72"/>
+      <c r="BJ5" s="72"/>
+      <c r="BK5" s="72"/>
+      <c r="BL5" s="72"/>
+      <c r="BM5" s="72"/>
+      <c r="BN5" s="72"/>
+      <c r="BO5" s="72"/>
+      <c r="BP5" s="72"/>
+      <c r="BQ5" s="72"/>
+      <c r="BR5" s="72"/>
+      <c r="BS5" s="72"/>
+      <c r="BT5" s="72"/>
+      <c r="BU5" s="72"/>
+      <c r="BV5" s="72"/>
+      <c r="BW5" s="72"/>
+      <c r="BX5" s="72"/>
+      <c r="BY5" s="72"/>
+      <c r="BZ5" s="72"/>
+      <c r="CA5" s="72"/>
+      <c r="CB5" s="72"/>
+      <c r="CC5" s="72"/>
+      <c r="CD5" s="72"/>
+      <c r="CE5" s="73"/>
       <c r="CF5" s="1"/>
     </row>
     <row r="6" spans="1:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="59">
+      <c r="G6" s="86">
         <v>45565</v>
       </c>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="59">
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="86">
         <f>G6+7</f>
         <v>45572</v>
       </c>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="62">
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="74">
         <f>N6+7</f>
         <v>45579</v>
       </c>
-      <c r="V6" s="60"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="60"/>
-      <c r="Y6" s="60"/>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="61"/>
-      <c r="AB6" s="62">
+      <c r="V6" s="72"/>
+      <c r="W6" s="72"/>
+      <c r="X6" s="72"/>
+      <c r="Y6" s="72"/>
+      <c r="Z6" s="72"/>
+      <c r="AA6" s="73"/>
+      <c r="AB6" s="74">
         <f>U6+7</f>
         <v>45586</v>
       </c>
-      <c r="AC6" s="60"/>
-      <c r="AD6" s="60"/>
-      <c r="AE6" s="60"/>
-      <c r="AF6" s="60"/>
-      <c r="AG6" s="60"/>
-      <c r="AH6" s="61"/>
-      <c r="AI6" s="62">
+      <c r="AC6" s="72"/>
+      <c r="AD6" s="72"/>
+      <c r="AE6" s="72"/>
+      <c r="AF6" s="72"/>
+      <c r="AG6" s="72"/>
+      <c r="AH6" s="73"/>
+      <c r="AI6" s="74">
         <f>AB6+7</f>
         <v>45593</v>
       </c>
-      <c r="AJ6" s="60"/>
-      <c r="AK6" s="60"/>
-      <c r="AL6" s="60"/>
-      <c r="AM6" s="60"/>
-      <c r="AN6" s="60"/>
-      <c r="AO6" s="61"/>
-      <c r="AP6" s="62">
+      <c r="AJ6" s="72"/>
+      <c r="AK6" s="72"/>
+      <c r="AL6" s="72"/>
+      <c r="AM6" s="72"/>
+      <c r="AN6" s="72"/>
+      <c r="AO6" s="73"/>
+      <c r="AP6" s="74">
         <f>AI6+7</f>
         <v>45600</v>
       </c>
-      <c r="AQ6" s="60"/>
-      <c r="AR6" s="60"/>
-      <c r="AS6" s="60"/>
-      <c r="AT6" s="60"/>
-      <c r="AU6" s="60"/>
-      <c r="AV6" s="61"/>
-      <c r="AW6" s="62">
+      <c r="AQ6" s="72"/>
+      <c r="AR6" s="72"/>
+      <c r="AS6" s="72"/>
+      <c r="AT6" s="72"/>
+      <c r="AU6" s="72"/>
+      <c r="AV6" s="73"/>
+      <c r="AW6" s="74">
         <f>AP6+7</f>
         <v>45607</v>
       </c>
-      <c r="AX6" s="60"/>
-      <c r="AY6" s="60"/>
-      <c r="AZ6" s="60"/>
-      <c r="BA6" s="60"/>
-      <c r="BB6" s="60"/>
-      <c r="BC6" s="61"/>
-      <c r="BD6" s="63">
+      <c r="AX6" s="72"/>
+      <c r="AY6" s="72"/>
+      <c r="AZ6" s="72"/>
+      <c r="BA6" s="72"/>
+      <c r="BB6" s="72"/>
+      <c r="BC6" s="73"/>
+      <c r="BD6" s="71">
         <f>AW6+7</f>
         <v>45614</v>
       </c>
-      <c r="BE6" s="60"/>
-      <c r="BF6" s="60"/>
-      <c r="BG6" s="60"/>
-      <c r="BH6" s="60"/>
-      <c r="BI6" s="60"/>
-      <c r="BJ6" s="61"/>
-      <c r="BK6" s="63">
+      <c r="BE6" s="72"/>
+      <c r="BF6" s="72"/>
+      <c r="BG6" s="72"/>
+      <c r="BH6" s="72"/>
+      <c r="BI6" s="72"/>
+      <c r="BJ6" s="73"/>
+      <c r="BK6" s="71">
         <f>BD6+7</f>
         <v>45621</v>
       </c>
-      <c r="BL6" s="60"/>
-      <c r="BM6" s="60"/>
-      <c r="BN6" s="60"/>
-      <c r="BO6" s="60"/>
-      <c r="BP6" s="60"/>
-      <c r="BQ6" s="61"/>
-      <c r="BR6" s="63">
+      <c r="BL6" s="72"/>
+      <c r="BM6" s="72"/>
+      <c r="BN6" s="72"/>
+      <c r="BO6" s="72"/>
+      <c r="BP6" s="72"/>
+      <c r="BQ6" s="73"/>
+      <c r="BR6" s="71">
         <f>BK6+7</f>
         <v>45628</v>
       </c>
-      <c r="BS6" s="60"/>
-      <c r="BT6" s="60"/>
-      <c r="BU6" s="60"/>
-      <c r="BV6" s="60"/>
-      <c r="BW6" s="60"/>
-      <c r="BX6" s="61"/>
-      <c r="BY6" s="63">
+      <c r="BS6" s="72"/>
+      <c r="BT6" s="72"/>
+      <c r="BU6" s="72"/>
+      <c r="BV6" s="72"/>
+      <c r="BW6" s="72"/>
+      <c r="BX6" s="73"/>
+      <c r="BY6" s="71">
         <f>BR6+7</f>
         <v>45635</v>
       </c>
-      <c r="BZ6" s="60"/>
-      <c r="CA6" s="60"/>
-      <c r="CB6" s="60"/>
-      <c r="CC6" s="60"/>
-      <c r="CD6" s="60"/>
-      <c r="CE6" s="61"/>
+      <c r="BZ6" s="72"/>
+      <c r="CA6" s="72"/>
+      <c r="CB6" s="72"/>
+      <c r="CC6" s="72"/>
+      <c r="CD6" s="72"/>
+      <c r="CE6" s="73"/>
       <c r="CF6" s="1"/>
     </row>
     <row r="7" spans="1:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
       <c r="G7" s="8" t="s">
         <v>12</v>
       </c>
@@ -2654,28 +2690,28 @@
       <c r="T16" s="27"/>
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
-      <c r="W16" s="77"/>
-      <c r="X16" s="77"/>
-      <c r="Y16" s="78"/>
-      <c r="Z16" s="78"/>
-      <c r="AA16" s="78"/>
-      <c r="AB16" s="79"/>
-      <c r="AC16" s="79"/>
-      <c r="AD16" s="79"/>
-      <c r="AE16" s="79"/>
-      <c r="AF16" s="79"/>
-      <c r="AG16" s="79"/>
-      <c r="AH16" s="79"/>
-      <c r="AI16" s="80"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
+      <c r="AG16" s="59"/>
+      <c r="AH16" s="59"/>
+      <c r="AI16" s="60"/>
       <c r="AJ16" s="44"/>
       <c r="AK16" s="44"/>
       <c r="AL16" s="44"/>
       <c r="AM16" s="44"/>
-      <c r="AN16" s="81"/>
-      <c r="AO16" s="81"/>
-      <c r="AP16" s="89"/>
-      <c r="AQ16" s="89"/>
-      <c r="AR16" s="89"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="61"/>
+      <c r="AP16" s="67"/>
+      <c r="AQ16" s="67"/>
+      <c r="AR16" s="67"/>
       <c r="AS16" s="33"/>
       <c r="AT16" s="33"/>
       <c r="AU16" s="33"/>
@@ -2687,12 +2723,12 @@
       <c r="BA16" s="44"/>
       <c r="BB16" s="44"/>
       <c r="BC16" s="44"/>
-      <c r="BD16" s="45"/>
-      <c r="BE16" s="45"/>
-      <c r="BF16" s="45"/>
-      <c r="BG16" s="45"/>
-      <c r="BH16" s="45"/>
-      <c r="BI16" s="45"/>
+      <c r="BD16" s="89"/>
+      <c r="BE16" s="89"/>
+      <c r="BF16" s="89"/>
+      <c r="BG16" s="34"/>
+      <c r="BH16" s="34"/>
+      <c r="BI16" s="34"/>
       <c r="BJ16" s="45"/>
       <c r="BK16" s="35"/>
       <c r="BL16" s="35"/>
@@ -2763,7 +2799,7 @@
       <c r="AF17" s="30"/>
       <c r="AG17" s="30"/>
       <c r="AH17" s="30"/>
-      <c r="AI17" s="80"/>
+      <c r="AI17" s="60"/>
       <c r="AJ17" s="44"/>
       <c r="AK17" s="44"/>
       <c r="AL17" s="44"/>
@@ -2848,12 +2884,12 @@
       <c r="T18" s="27"/>
       <c r="U18" s="28"/>
       <c r="V18" s="28"/>
-      <c r="W18" s="82"/>
-      <c r="X18" s="82"/>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="82"/>
-      <c r="AA18" s="82"/>
-      <c r="AB18" s="79"/>
+      <c r="W18" s="62"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="62"/>
+      <c r="AB18" s="59"/>
       <c r="AC18" s="30"/>
       <c r="AD18" s="30"/>
       <c r="AE18" s="30"/>
@@ -2883,9 +2919,9 @@
       <c r="BC18" s="44"/>
       <c r="BD18" s="45"/>
       <c r="BE18" s="45"/>
-      <c r="BF18" s="45"/>
-      <c r="BG18" s="45"/>
-      <c r="BH18" s="45"/>
+      <c r="BF18" s="89"/>
+      <c r="BG18" s="89"/>
+      <c r="BH18" s="89"/>
       <c r="BI18" s="45"/>
       <c r="BJ18" s="45"/>
       <c r="BK18" s="35"/>
@@ -2951,40 +2987,40 @@
       <c r="Z19" s="29"/>
       <c r="AA19" s="29"/>
       <c r="AB19" s="30"/>
-      <c r="AC19" s="79"/>
-      <c r="AD19" s="79"/>
-      <c r="AE19" s="79"/>
-      <c r="AF19" s="79"/>
-      <c r="AG19" s="79"/>
-      <c r="AH19" s="79"/>
-      <c r="AI19" s="77"/>
-      <c r="AJ19" s="77"/>
-      <c r="AK19" s="77"/>
-      <c r="AL19" s="77"/>
-      <c r="AM19" s="77"/>
-      <c r="AN19" s="77"/>
-      <c r="AO19" s="77"/>
-      <c r="AP19" s="88"/>
-      <c r="AQ19" s="88"/>
-      <c r="AR19" s="87"/>
-      <c r="AS19" s="87"/>
-      <c r="AT19" s="87"/>
-      <c r="AU19" s="87"/>
-      <c r="AV19" s="87"/>
-      <c r="AW19" s="85"/>
-      <c r="AX19" s="86"/>
-      <c r="AY19" s="86"/>
-      <c r="AZ19" s="86"/>
+      <c r="AC19" s="59"/>
+      <c r="AD19" s="59"/>
+      <c r="AE19" s="59"/>
+      <c r="AF19" s="59"/>
+      <c r="AG19" s="59"/>
+      <c r="AH19" s="59"/>
+      <c r="AI19" s="57"/>
+      <c r="AJ19" s="57"/>
+      <c r="AK19" s="57"/>
+      <c r="AL19" s="57"/>
+      <c r="AM19" s="57"/>
+      <c r="AN19" s="57"/>
+      <c r="AO19" s="57"/>
+      <c r="AP19" s="66"/>
+      <c r="AQ19" s="66"/>
+      <c r="AR19" s="65"/>
+      <c r="AS19" s="65"/>
+      <c r="AT19" s="65"/>
+      <c r="AU19" s="65"/>
+      <c r="AV19" s="65"/>
+      <c r="AW19" s="31"/>
+      <c r="AX19" s="32"/>
+      <c r="AY19" s="32"/>
+      <c r="AZ19" s="32"/>
       <c r="BA19" s="44"/>
       <c r="BB19" s="44"/>
       <c r="BC19" s="44"/>
       <c r="BD19" s="45"/>
       <c r="BE19" s="45"/>
       <c r="BF19" s="45"/>
-      <c r="BG19" s="45"/>
-      <c r="BH19" s="45"/>
-      <c r="BI19" s="45"/>
-      <c r="BJ19" s="45"/>
+      <c r="BG19" s="89"/>
+      <c r="BH19" s="89"/>
+      <c r="BI19" s="89"/>
+      <c r="BJ19" s="89"/>
       <c r="BK19" s="35"/>
       <c r="BL19" s="35"/>
       <c r="BM19" s="19"/>
@@ -3060,28 +3096,28 @@
       <c r="AL20" s="46"/>
       <c r="AM20" s="46"/>
       <c r="AN20" s="46"/>
-      <c r="AO20" s="90"/>
-      <c r="AP20" s="83"/>
-      <c r="AQ20" s="83"/>
-      <c r="AR20" s="83"/>
-      <c r="AS20" s="83"/>
-      <c r="AT20" s="83"/>
-      <c r="AU20" s="83"/>
-      <c r="AV20" s="83"/>
-      <c r="AW20" s="84"/>
-      <c r="AX20" s="84"/>
-      <c r="AY20" s="84"/>
-      <c r="AZ20" s="84"/>
-      <c r="BA20" s="84"/>
-      <c r="BB20" s="84"/>
-      <c r="BC20" s="84"/>
+      <c r="AO20" s="68"/>
+      <c r="AP20" s="63"/>
+      <c r="AQ20" s="63"/>
+      <c r="AR20" s="63"/>
+      <c r="AS20" s="63"/>
+      <c r="AT20" s="63"/>
+      <c r="AU20" s="63"/>
+      <c r="AV20" s="63"/>
+      <c r="AW20" s="64"/>
+      <c r="AX20" s="64"/>
+      <c r="AY20" s="64"/>
+      <c r="AZ20" s="64"/>
+      <c r="BA20" s="64"/>
+      <c r="BB20" s="64"/>
+      <c r="BC20" s="64"/>
       <c r="BD20" s="48"/>
       <c r="BE20" s="49"/>
       <c r="BF20" s="49"/>
       <c r="BG20" s="49"/>
       <c r="BH20" s="49"/>
-      <c r="BI20" s="45"/>
-      <c r="BJ20" s="45"/>
+      <c r="BI20" s="89"/>
+      <c r="BJ20" s="89"/>
       <c r="BK20" s="35"/>
       <c r="BL20" s="35"/>
       <c r="BM20" s="19"/>
@@ -3090,7 +3126,7 @@
       <c r="BP20" s="19"/>
       <c r="BQ20" s="19"/>
       <c r="BR20" s="34"/>
-      <c r="BS20" s="50"/>
+      <c r="BS20" s="34"/>
       <c r="BT20" s="50"/>
       <c r="BU20" s="50"/>
       <c r="BV20" s="50"/>
@@ -3163,22 +3199,22 @@
       <c r="AR21" s="47"/>
       <c r="AS21" s="47"/>
       <c r="AT21" s="47"/>
-      <c r="AU21" s="83"/>
-      <c r="AV21" s="83"/>
-      <c r="AW21" s="77"/>
-      <c r="AX21" s="77"/>
-      <c r="AY21" s="77"/>
-      <c r="AZ21" s="77"/>
-      <c r="BA21" s="77"/>
-      <c r="BB21" s="77"/>
-      <c r="BC21" s="77"/>
+      <c r="AU21" s="63"/>
+      <c r="AV21" s="63"/>
+      <c r="AW21" s="57"/>
+      <c r="AX21" s="57"/>
+      <c r="AY21" s="57"/>
+      <c r="AZ21" s="57"/>
+      <c r="BA21" s="57"/>
+      <c r="BB21" s="57"/>
+      <c r="BC21" s="57"/>
       <c r="BD21" s="48"/>
       <c r="BE21" s="49"/>
       <c r="BF21" s="49"/>
       <c r="BG21" s="49"/>
       <c r="BH21" s="49"/>
-      <c r="BI21" s="45"/>
-      <c r="BJ21" s="45"/>
+      <c r="BI21" s="89"/>
+      <c r="BJ21" s="89"/>
       <c r="BK21" s="35"/>
       <c r="BL21" s="35"/>
       <c r="BM21" s="19"/>
@@ -3186,8 +3222,8 @@
       <c r="BO21" s="19"/>
       <c r="BP21" s="19"/>
       <c r="BQ21" s="19"/>
-      <c r="BR21" s="34"/>
-      <c r="BS21" s="50"/>
+      <c r="BR21" s="94"/>
+      <c r="BS21" s="34"/>
       <c r="BT21" s="50"/>
       <c r="BU21" s="50"/>
       <c r="BV21" s="50"/>
@@ -3357,7 +3393,7 @@
       <c r="BA23" s="32"/>
       <c r="BB23" s="32"/>
       <c r="BC23" s="32"/>
-      <c r="BD23" s="34"/>
+      <c r="BD23" s="89"/>
       <c r="BE23" s="34"/>
       <c r="BF23" s="34"/>
       <c r="BG23" s="34"/>
@@ -3454,9 +3490,9 @@
       <c r="BA24" s="32"/>
       <c r="BB24" s="32"/>
       <c r="BC24" s="32"/>
-      <c r="BD24" s="34"/>
-      <c r="BE24" s="34"/>
-      <c r="BF24" s="34"/>
+      <c r="BD24" s="51"/>
+      <c r="BE24" s="89"/>
+      <c r="BF24" s="51"/>
       <c r="BG24" s="34"/>
       <c r="BH24" s="34"/>
       <c r="BI24" s="34"/>
@@ -3553,9 +3589,9 @@
       <c r="BC25" s="32"/>
       <c r="BD25" s="34"/>
       <c r="BE25" s="34"/>
-      <c r="BF25" s="34"/>
-      <c r="BG25" s="34"/>
-      <c r="BH25" s="34"/>
+      <c r="BF25" s="89"/>
+      <c r="BG25" s="89"/>
+      <c r="BH25" s="51"/>
       <c r="BI25" s="34"/>
       <c r="BJ25" s="34"/>
       <c r="BK25" s="35"/>
@@ -3652,9 +3688,9 @@
       <c r="BE26" s="51"/>
       <c r="BF26" s="51"/>
       <c r="BG26" s="51"/>
-      <c r="BH26" s="34"/>
-      <c r="BI26" s="34"/>
-      <c r="BJ26" s="34"/>
+      <c r="BH26" s="89"/>
+      <c r="BI26" s="89"/>
+      <c r="BJ26" s="89"/>
       <c r="BK26" s="35"/>
       <c r="BL26" s="35"/>
       <c r="BM26" s="19"/>
@@ -3750,8 +3786,8 @@
       <c r="BF27" s="34"/>
       <c r="BG27" s="34"/>
       <c r="BH27" s="51"/>
-      <c r="BI27" s="51"/>
-      <c r="BJ27" s="51"/>
+      <c r="BI27" s="89"/>
+      <c r="BJ27" s="89"/>
       <c r="BK27" s="26"/>
       <c r="BL27" s="26"/>
       <c r="BM27" s="19"/>
@@ -3759,7 +3795,7 @@
       <c r="BO27" s="19"/>
       <c r="BP27" s="19"/>
       <c r="BQ27" s="19"/>
-      <c r="BR27" s="34"/>
+      <c r="BR27" s="94"/>
       <c r="BS27" s="34"/>
       <c r="BT27" s="34"/>
       <c r="BU27" s="34"/>
@@ -3930,7 +3966,7 @@
       <c r="BA29" s="32"/>
       <c r="BB29" s="32"/>
       <c r="BC29" s="32"/>
-      <c r="BD29" s="34"/>
+      <c r="BD29" s="90"/>
       <c r="BE29" s="34"/>
       <c r="BF29" s="34"/>
       <c r="BG29" s="34"/>
@@ -4027,7 +4063,7 @@
       <c r="BA30" s="32"/>
       <c r="BB30" s="32"/>
       <c r="BC30" s="32"/>
-      <c r="BD30" s="34"/>
+      <c r="BD30" s="90"/>
       <c r="BE30" s="34"/>
       <c r="BF30" s="34"/>
       <c r="BG30" s="34"/>
@@ -4125,10 +4161,10 @@
       <c r="BB31" s="32"/>
       <c r="BC31" s="32"/>
       <c r="BD31" s="34"/>
-      <c r="BE31" s="34"/>
-      <c r="BF31" s="34"/>
-      <c r="BG31" s="34"/>
-      <c r="BH31" s="34"/>
+      <c r="BE31" s="90"/>
+      <c r="BF31" s="90"/>
+      <c r="BG31" s="90"/>
+      <c r="BH31" s="90"/>
       <c r="BI31" s="34"/>
       <c r="BJ31" s="34"/>
       <c r="BK31" s="35"/>
@@ -4226,16 +4262,16 @@
       <c r="BF32" s="51"/>
       <c r="BG32" s="51"/>
       <c r="BH32" s="34"/>
-      <c r="BI32" s="34"/>
-      <c r="BJ32" s="34"/>
-      <c r="BK32" s="35"/>
-      <c r="BL32" s="35"/>
+      <c r="BI32" s="90"/>
+      <c r="BJ32" s="90"/>
+      <c r="BK32" s="91"/>
+      <c r="BL32" s="91"/>
       <c r="BM32" s="19"/>
       <c r="BN32" s="19"/>
       <c r="BO32" s="19"/>
       <c r="BP32" s="19"/>
       <c r="BQ32" s="19"/>
-      <c r="BR32" s="34"/>
+      <c r="BR32" s="91"/>
       <c r="BS32" s="34"/>
       <c r="BT32" s="34"/>
       <c r="BU32" s="34"/>
@@ -4323,16 +4359,16 @@
       <c r="BF33" s="34"/>
       <c r="BG33" s="34"/>
       <c r="BH33" s="51"/>
-      <c r="BI33" s="51"/>
-      <c r="BJ33" s="51"/>
-      <c r="BK33" s="26"/>
-      <c r="BL33" s="26"/>
+      <c r="BI33" s="93"/>
+      <c r="BJ33" s="93"/>
+      <c r="BK33" s="94"/>
+      <c r="BL33" s="94"/>
       <c r="BM33" s="19"/>
       <c r="BN33" s="19"/>
       <c r="BO33" s="19"/>
       <c r="BP33" s="19"/>
       <c r="BQ33" s="19"/>
-      <c r="BR33" s="34"/>
+      <c r="BR33" s="94"/>
       <c r="BS33" s="34"/>
       <c r="BT33" s="34"/>
       <c r="BU33" s="34"/>
@@ -4503,15 +4539,15 @@
       <c r="BA35" s="52"/>
       <c r="BB35" s="52"/>
       <c r="BC35" s="52"/>
-      <c r="BD35" s="50"/>
-      <c r="BE35" s="50"/>
-      <c r="BF35" s="50"/>
-      <c r="BG35" s="50"/>
-      <c r="BH35" s="50"/>
+      <c r="BD35" s="92"/>
+      <c r="BE35" s="92"/>
+      <c r="BF35" s="34"/>
+      <c r="BG35" s="34"/>
+      <c r="BH35" s="34"/>
       <c r="BI35" s="34"/>
       <c r="BJ35" s="34"/>
-      <c r="BK35" s="35"/>
-      <c r="BL35" s="35"/>
+      <c r="BK35" s="53"/>
+      <c r="BL35" s="53"/>
       <c r="BM35" s="19"/>
       <c r="BN35" s="19"/>
       <c r="BO35" s="19"/>
@@ -4600,11 +4636,11 @@
       <c r="BA36" s="52"/>
       <c r="BB36" s="52"/>
       <c r="BC36" s="52"/>
-      <c r="BD36" s="50"/>
-      <c r="BE36" s="50"/>
-      <c r="BF36" s="50"/>
-      <c r="BG36" s="50"/>
-      <c r="BH36" s="50"/>
+      <c r="BD36" s="92"/>
+      <c r="BE36" s="34"/>
+      <c r="BF36" s="34"/>
+      <c r="BG36" s="34"/>
+      <c r="BH36" s="34"/>
       <c r="BI36" s="34"/>
       <c r="BJ36" s="34"/>
       <c r="BK36" s="35"/>
@@ -4700,10 +4736,10 @@
       <c r="BD37" s="50"/>
       <c r="BE37" s="50"/>
       <c r="BF37" s="50"/>
-      <c r="BG37" s="50"/>
-      <c r="BH37" s="50"/>
-      <c r="BI37" s="34"/>
-      <c r="BJ37" s="34"/>
+      <c r="BG37" s="92"/>
+      <c r="BH37" s="92"/>
+      <c r="BI37" s="90"/>
+      <c r="BJ37" s="90"/>
       <c r="BK37" s="35"/>
       <c r="BL37" s="35"/>
       <c r="BM37" s="19"/>
@@ -4712,7 +4748,7 @@
       <c r="BP37" s="19"/>
       <c r="BQ37" s="19"/>
       <c r="BR37" s="55"/>
-      <c r="BS37" s="55"/>
+      <c r="BS37" s="34"/>
       <c r="BT37" s="55"/>
       <c r="BU37" s="55"/>
       <c r="BV37" s="55"/>
@@ -4799,17 +4835,17 @@
       <c r="BF38" s="34"/>
       <c r="BG38" s="34"/>
       <c r="BH38" s="34"/>
-      <c r="BI38" s="34"/>
-      <c r="BJ38" s="34"/>
-      <c r="BK38" s="35"/>
-      <c r="BL38" s="35"/>
+      <c r="BI38" s="90"/>
+      <c r="BJ38" s="90"/>
+      <c r="BK38" s="91"/>
+      <c r="BL38" s="91"/>
       <c r="BM38" s="19"/>
       <c r="BN38" s="19"/>
       <c r="BO38" s="19"/>
       <c r="BP38" s="19"/>
       <c r="BQ38" s="19"/>
-      <c r="BR38" s="53"/>
-      <c r="BS38" s="53"/>
+      <c r="BR38" s="94"/>
+      <c r="BS38" s="34"/>
       <c r="BT38" s="53"/>
       <c r="BU38" s="53"/>
       <c r="BV38" s="53"/>
@@ -22788,23 +22824,23 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="BD5:CE5"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="U6:AA6"/>
+    <mergeCell ref="AB6:AH6"/>
+    <mergeCell ref="AI6:AO6"/>
+    <mergeCell ref="AP6:AV6"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="AA1:AH1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G5:T5"/>
+    <mergeCell ref="U5:BC5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="BY6:CE6"/>
     <mergeCell ref="AW6:BC6"/>
     <mergeCell ref="BD6:BJ6"/>
     <mergeCell ref="BK6:BQ6"/>
     <mergeCell ref="BR6:BX6"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="AA1:AH1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G5:T5"/>
-    <mergeCell ref="U5:BC5"/>
-    <mergeCell ref="BD5:CE5"/>
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="U6:AA6"/>
-    <mergeCell ref="AB6:AH6"/>
-    <mergeCell ref="AI6:AO6"/>
-    <mergeCell ref="AP6:AV6"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>

</xml_diff>